<commit_message>
Shrew 4 added, frames extracted and labeled, trained in colab
</commit_message>
<xml_diff>
--- a/shrew_retching_log.xlsx
+++ b/shrew_retching_log.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenstein/Desktop/shrew_emesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenstein/Desktop/ComputerVision/shrew_emesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{140523CC-1917-4F47-9F0C-E855A17759A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8BC0824-3CF0-A146-B3CF-DBB427B450DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16840" yWindow="6420" windowWidth="27640" windowHeight="16940" xr2:uid="{92F98C13-200D-AB43-9349-2C2B6CC8A24B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>Git Commit?</t>
+  </si>
+  <si>
+    <t>Added Shrew #4 with labels - very careful in labeling, excluded blurry images</t>
+  </si>
+  <si>
+    <t>Trained at 2000 iter pcutoff = 0.9, MSE ~5</t>
+  </si>
+  <si>
+    <t>labeled_data</t>
   </si>
 </sst>
 </file>
@@ -410,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{395509B2-5BB9-7145-916D-048A54EA4154}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -456,6 +465,22 @@
         <v>6</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>44497</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>